<commit_message>
Adición de módulo para pasar numeros a letras
</commit_message>
<xml_diff>
--- a/pytasks/Formatos/Ejemplo Calculo MATRIZ y Tazacion.xlsx
+++ b/pytasks/Formatos/Ejemplo Calculo MATRIZ y Tazacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pollo\OneDrive\Development\1-BienesFuturos\pytasks\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C706F9-B5B0-4223-90D6-BA9E6749D29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA6E894-34B6-486F-8919-6DBCADEA8F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="1905" windowWidth="21600" windowHeight="11505" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="2880" windowWidth="21600" windowHeight="11505" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRIZ" sheetId="3" r:id="rId1"/>
@@ -780,6 +780,7 @@
     <xf numFmtId="43" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -801,7 +802,6 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1182,7 +1182,7 @@
       <selection activeCell="AA81" sqref="AA81"/>
       <selection pane="topRight" activeCell="AA81" sqref="AA81"/>
       <selection pane="bottomLeft" activeCell="AA81" sqref="AA81"/>
-      <selection pane="bottomRight" activeCell="T13" sqref="T13"/>
+      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1302,11 +1302,11 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="86">
+      <c r="D7" s="87">
         <f>+MAX(MATRIZ!$AA$12:$AA$12)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2"/>
       <c r="L7" s="8"/>
@@ -1354,32 +1354,32 @@
       <c r="B10" s="2"/>
       <c r="D10" s="9"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="83" t="s">
+      <c r="F10" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="80" t="s">
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="82"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="82"/>
+      <c r="X10" s="82"/>
+      <c r="Y10" s="82"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="83"/>
     </row>
     <row r="11" spans="1:33" s="28" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
@@ -1704,7 +1704,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="18"/>
-      <c r="R15" s="87" t="s">
+      <c r="R15" s="80" t="s">
         <v>54</v>
       </c>
       <c r="S15" s="11">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E16" s="42"/>
       <c r="G16" s="16"/>
-      <c r="R16" s="87">
+      <c r="R16" s="80">
         <v>0.3</v>
       </c>
       <c r="T16" s="11" t="s">

</xml_diff>